<commit_message>
actualización del archivo de noticias hasta el 24 de septiembrev2
</commit_message>
<xml_diff>
--- a/noticias_fondo con todas las fuentes_rango_03-07-2025.xlsx
+++ b/noticias_fondo con todas las fuentes_rango_03-07-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8AD2A2-23F3-4E3C-874B-3502235A4CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7D4E93-43A2-4791-9CDF-5368BD248838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{225F6CCB-45F1-4943-BB05-93453F413104}"/>
   </bookViews>
@@ -9114,8 +9114,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:N1076"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F1063" sqref="F1063"/>
+    <sheetView tabSelected="1" topLeftCell="A1044" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D1076"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>